<commit_message>
Imágenes finales (A) | Momentos de Hu - original
</commit_message>
<xml_diff>
--- a/Files/Momentos_Hu.xlsx
+++ b/Files/Momentos_Hu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\areyc\OneDrive\DOCS\Escritorio\2021\Proyectos\Kivy\pdi-python\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886A2707-2C53-4353-AFD5-0F3FBAD355A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE4624A-BE69-417B-98CD-FEAD5BD45F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -142,13 +142,16 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Rotada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +169,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -206,10 +217,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,6 +484,50 @@
         <a:xfrm>
           <a:off x="8896351" y="22926676"/>
           <a:ext cx="838198" cy="838198"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>157575</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>153120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E65AF25E-D4CB-4580-125E-9EC0DB5A9612}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9963149" y="22926676"/>
+          <a:ext cx="757651" cy="848444"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -747,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:T132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="T127" sqref="T127"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +963,7 @@
         <v>11</v>
       </c>
       <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+      <c r="N9" s="3"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
@@ -3117,14 +3174,30 @@
       <c r="L128" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M128" s="1"/>
-      <c r="N128" s="1"/>
-      <c r="O128" s="1"/>
-      <c r="P128" s="1"/>
-      <c r="Q128" s="1"/>
-      <c r="R128" s="1"/>
-      <c r="S128" s="1"/>
-      <c r="T128" s="1"/>
+      <c r="M128" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N128" s="1">
+        <v>3.0760000000000001</v>
+      </c>
+      <c r="O128" s="1">
+        <v>6.9779999999999998</v>
+      </c>
+      <c r="P128" s="1">
+        <v>9.6950000000000003</v>
+      </c>
+      <c r="Q128" s="1">
+        <v>12.823</v>
+      </c>
+      <c r="R128" s="1">
+        <v>-24.167000000000002</v>
+      </c>
+      <c r="S128" s="1">
+        <v>17.213000000000001</v>
+      </c>
+      <c r="T128" s="1">
+        <v>-24.329000000000001</v>
+      </c>
     </row>
     <row r="129" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="s">

</xml_diff>